<commit_message>
first version (csv-export completed)
</commit_message>
<xml_diff>
--- a/migraine_diary_data_definition.xlsx
+++ b/migraine_diary_data_definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\JavaWorkspaces\migraine_diary\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>get_up</t>
   </si>
@@ -147,15 +147,6 @@
   </si>
   <si>
     <t>Painkiller</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Zahlen einfügen</t>
-  </si>
-  <si>
-    <t>TODO:</t>
   </si>
   <si>
     <t>surplus_protein</t>
@@ -484,7 +475,7 @@
   <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,22 +497,22 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -530,7 +521,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K1" t="s">
         <v>9</v>
@@ -564,23 +555,23 @@
       <c r="A2" s="1">
         <v>41275</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="2">
-        <v>5</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>15</v>
@@ -623,20 +614,20 @@
       <c r="V2" s="2"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -659,19 +650,19 @@
       <c r="V3" s="2"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -691,15 +682,13 @@
       <c r="V4" s="2"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -717,12 +706,10 @@
       <c r="V5" s="2"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -782,18 +769,10 @@
       <c r="V8" s="2"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -811,8 +790,6 @@
       <c r="V9" s="2"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -832,10 +809,6 @@
       <c r="V10" s="2"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -853,10 +826,6 @@
       <c r="V11" s="2"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -874,10 +843,6 @@
       <c r="V12" s="2"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -895,10 +860,6 @@
       <c r="V13" s="2"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -918,8 +879,6 @@
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>

</xml_diff>

<commit_message>
finalized app for version 0.1
</commit_message>
<xml_diff>
--- a/migraine_diary_data_definition.xlsx
+++ b/migraine_diary_data_definition.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>get_up</t>
   </si>
@@ -68,12 +68,6 @@
     <t>weather</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>sunny</t>
   </si>
   <si>
@@ -116,24 +110,12 @@
     <t>temp</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>INT</t>
-  </si>
-  <si>
     <t>sports_endurance</t>
   </si>
   <si>
     <t>sports_power</t>
   </si>
   <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>TEXT</t>
-  </si>
-  <si>
     <t>headpain</t>
   </si>
   <si>
@@ -153,14 +135,28 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
+    <t>STRING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -188,10 +184,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -475,7 +473,7 @@
   <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +485,7 @@
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -509,10 +507,10 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -521,7 +519,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K1" t="s">
         <v>9</v>
@@ -539,16 +537,13 @@
         <v>13</v>
       </c>
       <c r="P1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" t="s">
         <v>29</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -562,72 +557,70 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="P2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -637,11 +630,9 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -651,17 +642,17 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -671,7 +662,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -683,11 +674,11 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -707,7 +698,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2"/>
       <c r="H6" s="2"/>

</xml_diff>